<commit_message>
add keys and totals
</commit_message>
<xml_diff>
--- a/haas/output_csv/haas_emissions_report.xlsx
+++ b/haas/output_csv/haas_emissions_report.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,1237 +424,2271 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>event-time</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>event-location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>event-catering</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>event-attendance</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>student-train</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>student-car</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>student-plane</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>student-bus</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>student-bike</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>student-total</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
         <is>
           <t>nonstudent-train</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>nonstudent-car</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>nonstudent-plane</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>nonstudent-bus</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>nonstudent-bike</t>
         </is>
       </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>nonstudent-total</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>total-emissions</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2023-08-05T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Haas - Café Think - Chou Hall</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Bancroft</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>205</v>
+      </c>
+      <c r="E2" t="n">
         <v>7.806400000000001</v>
       </c>
-      <c r="B2" t="n">
+      <c r="F2" t="n">
         <v>181.39425</v>
       </c>
-      <c r="C2" t="n">
+      <c r="G2" t="n">
         <v>241.5105</v>
       </c>
-      <c r="D2" t="n">
+      <c r="H2" t="n">
         <v>23.1316875</v>
       </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>453.8428375</v>
+      </c>
+      <c r="K2" t="n">
         <v>0.6888000000000001</v>
       </c>
-      <c r="G2" t="n">
+      <c r="L2" t="n">
         <v>65.08852499999999</v>
       </c>
-      <c r="H2" t="n">
+      <c r="M2" t="n">
         <v>213.0975</v>
       </c>
-      <c r="I2" t="n">
+      <c r="N2" t="n">
         <v>1.632825</v>
       </c>
-      <c r="J2" t="n">
-        <v>0</v>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>280.50765</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>734.3504875</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2023-08-12T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Haas - Café Think - Chou Hall</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Bancroft</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>279</v>
+      </c>
+      <c r="E3" t="n">
         <v>10.62432</v>
       </c>
-      <c r="B3" t="n">
+      <c r="F3" t="n">
         <v>246.87315</v>
       </c>
-      <c r="C3" t="n">
+      <c r="G3" t="n">
         <v>328.6899</v>
       </c>
-      <c r="D3" t="n">
+      <c r="H3" t="n">
         <v>31.4816625</v>
       </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>617.6690325</v>
+      </c>
+      <c r="K3" t="n">
         <v>0.9374400000000002</v>
       </c>
-      <c r="G3" t="n">
+      <c r="L3" t="n">
         <v>88.583895</v>
       </c>
-      <c r="H3" t="n">
+      <c r="M3" t="n">
         <v>290.0205</v>
       </c>
-      <c r="I3" t="n">
+      <c r="N3" t="n">
         <v>2.222235</v>
       </c>
-      <c r="J3" t="n">
-        <v>0</v>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>381.76407</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>999.4331024999999</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023-08-19T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Haas - Café Think - Chou Hall</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Bancroft</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>305</v>
+      </c>
+      <c r="E4" t="n">
         <v>6.832000000000002</v>
       </c>
-      <c r="B4" t="n">
+      <c r="F4" t="n">
         <v>158.7525</v>
       </c>
-      <c r="C4" t="n">
+      <c r="G4" t="n">
         <v>211.365</v>
       </c>
-      <c r="D4" t="n">
+      <c r="H4" t="n">
         <v>20.244375</v>
       </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>397.193875</v>
+      </c>
+      <c r="K4" t="n">
         <v>3.416000000000001</v>
       </c>
-      <c r="G4" t="n">
+      <c r="L4" t="n">
         <v>322.79675</v>
       </c>
-      <c r="H4" t="n">
+      <c r="M4" t="n">
         <v>1056.825</v>
       </c>
-      <c r="I4" t="n">
+      <c r="N4" t="n">
         <v>8.09775</v>
       </c>
-      <c r="J4" t="n">
-        <v>0</v>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>1391.1355</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>1788.329375</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023-08-26T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Haas - Café Think - Chou Hall</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Bancroft</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>309</v>
+      </c>
+      <c r="E5" t="n">
         <v>9.690239999999999</v>
       </c>
-      <c r="B5" t="n">
+      <c r="F5" t="n">
         <v>225.1682999999999</v>
       </c>
-      <c r="C5" t="n">
+      <c r="G5" t="n">
         <v>299.7918</v>
       </c>
-      <c r="D5" t="n">
+      <c r="H5" t="n">
         <v>28.713825</v>
       </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>563.364165</v>
+      </c>
+      <c r="K5" t="n">
         <v>2.07648</v>
       </c>
-      <c r="G5" t="n">
+      <c r="L5" t="n">
         <v>196.21809</v>
       </c>
-      <c r="H5" t="n">
+      <c r="M5" t="n">
         <v>642.4110000000001</v>
       </c>
-      <c r="I5" t="n">
+      <c r="N5" t="n">
         <v>4.92237</v>
       </c>
-      <c r="J5" t="n">
-        <v>0</v>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>845.6279400000001</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1408.992105</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2023-12-02T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Haas - Café Think - Chou Hall</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Bancroft</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>196</v>
+      </c>
+      <c r="E6" t="n">
         <v>7.024640000000001</v>
       </c>
-      <c r="B6" t="n">
+      <c r="F6" t="n">
         <v>163.2288</v>
       </c>
-      <c r="C6" t="n">
+      <c r="G6" t="n">
         <v>217.3248</v>
       </c>
-      <c r="D6" t="n">
+      <c r="H6" t="n">
         <v>20.8152</v>
       </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>408.39344</v>
+      </c>
+      <c r="K6" t="n">
         <v>0.8780800000000001</v>
       </c>
-      <c r="G6" t="n">
+      <c r="L6" t="n">
         <v>82.97464000000001</v>
       </c>
-      <c r="H6" t="n">
+      <c r="M6" t="n">
         <v>271.656</v>
       </c>
-      <c r="I6" t="n">
+      <c r="N6" t="n">
         <v>2.08152</v>
       </c>
-      <c r="J6" t="n">
-        <v>0</v>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>357.5902400000001</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>765.98368</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2023-09-09T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Haas - Café Think - Chou Hall</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Bancroft</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>332</v>
+      </c>
+      <c r="E7" t="n">
         <v>12.64256</v>
       </c>
-      <c r="B7" t="n">
+      <c r="F7" t="n">
         <v>293.7702</v>
       </c>
-      <c r="C7" t="n">
+      <c r="G7" t="n">
         <v>391.1292</v>
       </c>
-      <c r="D7" t="n">
+      <c r="H7" t="n">
         <v>37.46205</v>
       </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>735.00401</v>
+      </c>
+      <c r="K7" t="n">
         <v>1.11552</v>
       </c>
-      <c r="G7" t="n">
+      <c r="L7" t="n">
         <v>105.41166</v>
       </c>
-      <c r="H7" t="n">
+      <c r="M7" t="n">
         <v>345.114</v>
       </c>
-      <c r="I7" t="n">
+      <c r="N7" t="n">
         <v>2.64438</v>
       </c>
-      <c r="J7" t="n">
-        <v>0</v>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>454.28556</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>1189.28957</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2023-09-16T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Haas - Café Think - Chou Hall</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Bancroft</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>296</v>
+      </c>
+      <c r="E8" t="n">
         <v>11.27168</v>
       </c>
-      <c r="B8" t="n">
+      <c r="F8" t="n">
         <v>261.9155999999999</v>
       </c>
-      <c r="C8" t="n">
+      <c r="G8" t="n">
         <v>348.7176</v>
       </c>
-      <c r="D8" t="n">
+      <c r="H8" t="n">
         <v>33.3999</v>
       </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>655.3047799999999</v>
+      </c>
+      <c r="K8" t="n">
         <v>0.9945600000000001</v>
       </c>
-      <c r="G8" t="n">
+      <c r="L8" t="n">
         <v>93.98147999999999</v>
       </c>
-      <c r="H8" t="n">
+      <c r="M8" t="n">
         <v>307.692</v>
       </c>
-      <c r="I8" t="n">
+      <c r="N8" t="n">
         <v>2.35764</v>
       </c>
-      <c r="J8" t="n">
-        <v>0</v>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>405.02568</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>1060.33046</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2023-09-23T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Haas - Café Think - Chou Hall</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Bancroft</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>303</v>
+      </c>
+      <c r="E9" t="n">
         <v>6.787200000000001</v>
       </c>
-      <c r="B9" t="n">
+      <c r="F9" t="n">
         <v>157.7115</v>
       </c>
-      <c r="C9" t="n">
+      <c r="G9" t="n">
         <v>209.979</v>
       </c>
-      <c r="D9" t="n">
+      <c r="H9" t="n">
         <v>20.111625</v>
       </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>394.589325</v>
+      </c>
+      <c r="K9" t="n">
         <v>3.393600000000001</v>
       </c>
-      <c r="G9" t="n">
+      <c r="L9" t="n">
         <v>320.6800499999999</v>
       </c>
-      <c r="H9" t="n">
+      <c r="M9" t="n">
         <v>1049.895</v>
       </c>
-      <c r="I9" t="n">
+      <c r="N9" t="n">
         <v>8.044650000000001</v>
       </c>
-      <c r="J9" t="n">
-        <v>0</v>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>1382.0133</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>1776.602625</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2023-09-30T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Haas - Café Think - Chou Hall</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Bancroft</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>314</v>
+      </c>
+      <c r="E10" t="n">
         <v>9.847040000000002</v>
       </c>
-      <c r="B10" t="n">
+      <c r="F10" t="n">
         <v>228.8118</v>
       </c>
-      <c r="C10" t="n">
+      <c r="G10" t="n">
         <v>304.6428</v>
       </c>
-      <c r="D10" t="n">
+      <c r="H10" t="n">
         <v>29.17845</v>
       </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>572.4800899999999</v>
+      </c>
+      <c r="K10" t="n">
         <v>2.11008</v>
       </c>
-      <c r="G10" t="n">
+      <c r="L10" t="n">
         <v>199.39314</v>
       </c>
-      <c r="H10" t="n">
+      <c r="M10" t="n">
         <v>652.8059999999999</v>
       </c>
-      <c r="I10" t="n">
+      <c r="N10" t="n">
         <v>5.00202</v>
       </c>
-      <c r="J10" t="n">
-        <v>0</v>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>859.3112399999999</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>1431.79133</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-02-01T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SPIEKER FORUM</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ACT</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>180</v>
+      </c>
+      <c r="E11" t="n">
         <v>6.4512</v>
       </c>
-      <c r="B11" t="n">
+      <c r="F11" t="n">
         <v>149.904</v>
       </c>
-      <c r="C11" t="n">
+      <c r="G11" t="n">
         <v>199.584</v>
       </c>
-      <c r="D11" t="n">
+      <c r="H11" t="n">
         <v>19.116</v>
       </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>375.0551999999999</v>
+      </c>
+      <c r="K11" t="n">
         <v>0.8064</v>
       </c>
-      <c r="G11" t="n">
+      <c r="L11" t="n">
         <v>76.2012</v>
       </c>
-      <c r="H11" t="n">
+      <c r="M11" t="n">
         <v>249.48</v>
       </c>
-      <c r="I11" t="n">
+      <c r="N11" t="n">
         <v>1.9116</v>
       </c>
-      <c r="J11" t="n">
-        <v>0</v>
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" t="n">
+        <v>328.3992</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>703.4543999999999</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-02-07T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SPIEKER FORUM</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ACT</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>180</v>
+      </c>
+      <c r="E12" t="n">
         <v>6.854400000000001</v>
       </c>
-      <c r="B12" t="n">
+      <c r="F12" t="n">
         <v>159.273</v>
       </c>
-      <c r="C12" t="n">
+      <c r="G12" t="n">
         <v>212.058</v>
       </c>
-      <c r="D12" t="n">
+      <c r="H12" t="n">
         <v>20.31075</v>
       </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="n">
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>398.4961499999999</v>
+      </c>
+      <c r="K12" t="n">
         <v>0.6048000000000001</v>
       </c>
-      <c r="G12" t="n">
+      <c r="L12" t="n">
         <v>57.15089999999999</v>
       </c>
-      <c r="H12" t="n">
+      <c r="M12" t="n">
         <v>187.11</v>
       </c>
-      <c r="I12" t="n">
+      <c r="N12" t="n">
         <v>1.4337</v>
       </c>
-      <c r="J12" t="n">
-        <v>0</v>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>246.2994</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>644.7955499999999</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-03-11T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SPIEKER FORUM</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ACT</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>180</v>
+      </c>
+      <c r="E13" t="n">
         <v>6.854400000000001</v>
       </c>
-      <c r="B13" t="n">
+      <c r="F13" t="n">
         <v>159.273</v>
       </c>
-      <c r="C13" t="n">
+      <c r="G13" t="n">
         <v>212.058</v>
       </c>
-      <c r="D13" t="n">
+      <c r="H13" t="n">
         <v>20.31075</v>
       </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" t="n">
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>398.4961499999999</v>
+      </c>
+      <c r="K13" t="n">
         <v>0.6048000000000001</v>
       </c>
-      <c r="G13" t="n">
+      <c r="L13" t="n">
         <v>57.15089999999999</v>
       </c>
-      <c r="H13" t="n">
+      <c r="M13" t="n">
         <v>187.11</v>
       </c>
-      <c r="I13" t="n">
+      <c r="N13" t="n">
         <v>1.4337</v>
       </c>
-      <c r="J13" t="n">
-        <v>0</v>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" t="n">
+        <v>246.2994</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>644.7955499999999</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-04-02T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SPIEKER FORUM</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>ACT</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>180</v>
+      </c>
+      <c r="E14" t="n">
         <v>4.032000000000001</v>
       </c>
-      <c r="B14" t="n">
+      <c r="F14" t="n">
         <v>93.69</v>
       </c>
-      <c r="C14" t="n">
+      <c r="G14" t="n">
         <v>124.74</v>
       </c>
-      <c r="D14" t="n">
+      <c r="H14" t="n">
         <v>11.9475</v>
       </c>
-      <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="n">
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>234.4095</v>
+      </c>
+      <c r="K14" t="n">
         <v>2.016</v>
       </c>
-      <c r="G14" t="n">
+      <c r="L14" t="n">
         <v>190.503</v>
       </c>
-      <c r="H14" t="n">
+      <c r="M14" t="n">
         <v>623.6999999999999</v>
       </c>
-      <c r="I14" t="n">
+      <c r="N14" t="n">
         <v>4.779</v>
       </c>
-      <c r="J14" t="n">
-        <v>0</v>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>820.9979999999999</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>1055.4075</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-04-04T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SPIEKER FORUM</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ACT</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>180</v>
+      </c>
+      <c r="E15" t="n">
         <v>5.644799999999999</v>
       </c>
-      <c r="B15" t="n">
+      <c r="F15" t="n">
         <v>131.166</v>
       </c>
-      <c r="C15" t="n">
+      <c r="G15" t="n">
         <v>174.636</v>
       </c>
-      <c r="D15" t="n">
+      <c r="H15" t="n">
         <v>16.7265</v>
       </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" t="n">
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>328.1732999999999</v>
+      </c>
+      <c r="K15" t="n">
         <v>1.2096</v>
       </c>
-      <c r="G15" t="n">
+      <c r="L15" t="n">
         <v>114.3018</v>
       </c>
-      <c r="H15" t="n">
+      <c r="M15" t="n">
         <v>374.22</v>
       </c>
-      <c r="I15" t="n">
+      <c r="N15" t="n">
         <v>2.8674</v>
       </c>
-      <c r="J15" t="n">
-        <v>0</v>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>492.5988</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>820.7720999999999</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-04-16T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SPIEKER FORUM</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ACT</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>170</v>
+      </c>
+      <c r="E16" t="n">
         <v>6.092800000000001</v>
       </c>
-      <c r="B16" t="n">
+      <c r="F16" t="n">
         <v>141.576</v>
       </c>
-      <c r="C16" t="n">
+      <c r="G16" t="n">
         <v>188.496</v>
       </c>
-      <c r="D16" t="n">
+      <c r="H16" t="n">
         <v>18.054</v>
       </c>
-      <c r="E16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" t="n">
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>354.2188</v>
+      </c>
+      <c r="K16" t="n">
         <v>0.7616000000000002</v>
       </c>
-      <c r="G16" t="n">
+      <c r="L16" t="n">
         <v>71.96779999999998</v>
       </c>
-      <c r="H16" t="n">
+      <c r="M16" t="n">
         <v>235.62</v>
       </c>
-      <c r="I16" t="n">
+      <c r="N16" t="n">
         <v>1.8054</v>
       </c>
-      <c r="J16" t="n">
-        <v>0</v>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" t="n">
+        <v>310.1548</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>664.3736</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2023-11-01T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>SPIEKER FORUM</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>ACT</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>180</v>
+      </c>
+      <c r="E17" t="n">
         <v>6.854400000000001</v>
       </c>
-      <c r="B17" t="n">
+      <c r="F17" t="n">
         <v>159.273</v>
       </c>
-      <c r="C17" t="n">
+      <c r="G17" t="n">
         <v>212.058</v>
       </c>
-      <c r="D17" t="n">
+      <c r="H17" t="n">
         <v>20.31075</v>
       </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" t="n">
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>398.4961499999999</v>
+      </c>
+      <c r="K17" t="n">
         <v>0.6048000000000001</v>
       </c>
-      <c r="G17" t="n">
+      <c r="L17" t="n">
         <v>57.15089999999999</v>
       </c>
-      <c r="H17" t="n">
+      <c r="M17" t="n">
         <v>187.11</v>
       </c>
-      <c r="I17" t="n">
+      <c r="N17" t="n">
         <v>1.4337</v>
       </c>
-      <c r="J17" t="n">
-        <v>0</v>
+      <c r="O17" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" t="n">
+        <v>246.2994</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>644.7955499999999</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2023-11-08T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SPIEKER FORUM</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>ACT</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>180</v>
+      </c>
+      <c r="E18" t="n">
         <v>6.854400000000001</v>
       </c>
-      <c r="B18" t="n">
+      <c r="F18" t="n">
         <v>159.273</v>
       </c>
-      <c r="C18" t="n">
+      <c r="G18" t="n">
         <v>212.058</v>
       </c>
-      <c r="D18" t="n">
+      <c r="H18" t="n">
         <v>20.31075</v>
       </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" t="n">
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>398.4961499999999</v>
+      </c>
+      <c r="K18" t="n">
         <v>0.6048000000000001</v>
       </c>
-      <c r="G18" t="n">
+      <c r="L18" t="n">
         <v>57.15089999999999</v>
       </c>
-      <c r="H18" t="n">
+      <c r="M18" t="n">
         <v>187.11</v>
       </c>
-      <c r="I18" t="n">
+      <c r="N18" t="n">
         <v>1.4337</v>
       </c>
-      <c r="J18" t="n">
-        <v>0</v>
+      <c r="O18" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" t="n">
+        <v>246.2994</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>644.7955499999999</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-02-21T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>132 Cheit Hall</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>ACT</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>50</v>
+      </c>
+      <c r="E19" t="n">
         <v>1.12</v>
       </c>
-      <c r="B19" t="n">
+      <c r="F19" t="n">
         <v>26.025</v>
       </c>
-      <c r="C19" t="n">
+      <c r="G19" t="n">
         <v>34.65</v>
       </c>
-      <c r="D19" t="n">
+      <c r="H19" t="n">
         <v>3.31875</v>
       </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" t="n">
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>65.11375</v>
+      </c>
+      <c r="K19" t="n">
         <v>0.5600000000000001</v>
       </c>
-      <c r="G19" t="n">
+      <c r="L19" t="n">
         <v>52.9175</v>
       </c>
-      <c r="H19" t="n">
+      <c r="M19" t="n">
         <v>173.25</v>
       </c>
-      <c r="I19" t="n">
+      <c r="N19" t="n">
         <v>1.3275</v>
       </c>
-      <c r="J19" t="n">
-        <v>0</v>
+      <c r="O19" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" t="n">
+        <v>228.055</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>293.16875</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2023-04-02T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SPIEKER FORUM</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>ACT</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>125</v>
+      </c>
+      <c r="E20" t="n">
         <v>3.92</v>
       </c>
-      <c r="B20" t="n">
+      <c r="F20" t="n">
         <v>91.08749999999999</v>
       </c>
-      <c r="C20" t="n">
+      <c r="G20" t="n">
         <v>121.275</v>
       </c>
-      <c r="D20" t="n">
+      <c r="H20" t="n">
         <v>11.615625</v>
       </c>
-      <c r="E20" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" t="n">
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>227.898125</v>
+      </c>
+      <c r="K20" t="n">
         <v>0.8400000000000001</v>
       </c>
-      <c r="G20" t="n">
+      <c r="L20" t="n">
         <v>79.37625</v>
       </c>
-      <c r="H20" t="n">
+      <c r="M20" t="n">
         <v>259.875</v>
       </c>
-      <c r="I20" t="n">
+      <c r="N20" t="n">
         <v>1.99125</v>
       </c>
-      <c r="J20" t="n">
-        <v>0</v>
+      <c r="O20" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" t="n">
+        <v>342.0825</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>569.9806249999999</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2023-12-08T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Wells Fargo Room</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ACT</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>30</v>
+      </c>
+      <c r="E21" t="n">
         <v>1.0752</v>
       </c>
-      <c r="B21" t="n">
+      <c r="F21" t="n">
         <v>24.98399999999999</v>
       </c>
-      <c r="C21" t="n">
+      <c r="G21" t="n">
         <v>33.264</v>
       </c>
-      <c r="D21" t="n">
+      <c r="H21" t="n">
         <v>3.186</v>
       </c>
-      <c r="E21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" t="n">
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>62.50919999999999</v>
+      </c>
+      <c r="K21" t="n">
         <v>0.1344</v>
       </c>
-      <c r="G21" t="n">
+      <c r="L21" t="n">
         <v>12.7002</v>
       </c>
-      <c r="H21" t="n">
+      <c r="M21" t="n">
         <v>41.58000000000001</v>
       </c>
-      <c r="I21" t="n">
+      <c r="N21" t="n">
         <v>0.3185999999999999</v>
       </c>
-      <c r="J21" t="n">
-        <v>0</v>
+      <c r="O21" t="n">
+        <v>0</v>
+      </c>
+      <c r="P21" t="n">
+        <v>54.7332</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>117.2424</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2023-11-08T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Wells Fargo Room</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>ACT</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>50</v>
+      </c>
+      <c r="E22" t="n">
         <v>1.904</v>
       </c>
-      <c r="B22" t="n">
+      <c r="F22" t="n">
         <v>44.2425</v>
       </c>
-      <c r="C22" t="n">
+      <c r="G22" t="n">
         <v>58.90499999999999</v>
       </c>
-      <c r="D22" t="n">
+      <c r="H22" t="n">
         <v>5.641875</v>
       </c>
-      <c r="E22" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" t="n">
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>110.693375</v>
+      </c>
+      <c r="K22" t="n">
         <v>0.168</v>
       </c>
-      <c r="G22" t="n">
+      <c r="L22" t="n">
         <v>15.87525</v>
       </c>
-      <c r="H22" t="n">
+      <c r="M22" t="n">
         <v>51.97499999999999</v>
       </c>
-      <c r="I22" t="n">
+      <c r="N22" t="n">
         <v>0.3982499999999999</v>
       </c>
-      <c r="J22" t="n">
-        <v>0</v>
+      <c r="O22" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" t="n">
+        <v>68.4165</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>179.109875</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2023-01-24T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>SPIEKER FORUM</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>ACT</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>160</v>
+      </c>
+      <c r="E23" t="n">
         <v>6.092800000000001</v>
       </c>
-      <c r="B23" t="n">
+      <c r="F23" t="n">
         <v>141.576</v>
       </c>
-      <c r="C23" t="n">
+      <c r="G23" t="n">
         <v>188.496</v>
       </c>
-      <c r="D23" t="n">
+      <c r="H23" t="n">
         <v>18.054</v>
       </c>
-      <c r="E23" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" t="n">
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>354.2188</v>
+      </c>
+      <c r="K23" t="n">
         <v>0.5376000000000001</v>
       </c>
-      <c r="G23" t="n">
+      <c r="L23" t="n">
         <v>50.8008</v>
       </c>
-      <c r="H23" t="n">
+      <c r="M23" t="n">
         <v>166.32</v>
       </c>
-      <c r="I23" t="n">
+      <c r="N23" t="n">
         <v>1.2744</v>
       </c>
-      <c r="J23" t="n">
-        <v>0</v>
+      <c r="O23" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" t="n">
+        <v>218.9328</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>573.1516</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2023-03-23T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>SPIEKER FORUM</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ACT</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>180</v>
+      </c>
+      <c r="E24" t="n">
         <v>4.032000000000001</v>
       </c>
-      <c r="B24" t="n">
+      <c r="F24" t="n">
         <v>93.69</v>
       </c>
-      <c r="C24" t="n">
+      <c r="G24" t="n">
         <v>124.74</v>
       </c>
-      <c r="D24" t="n">
+      <c r="H24" t="n">
         <v>11.9475</v>
       </c>
-      <c r="E24" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" t="n">
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="n">
+        <v>234.4095</v>
+      </c>
+      <c r="K24" t="n">
         <v>2.016</v>
       </c>
-      <c r="G24" t="n">
+      <c r="L24" t="n">
         <v>190.503</v>
       </c>
-      <c r="H24" t="n">
+      <c r="M24" t="n">
         <v>623.6999999999999</v>
       </c>
-      <c r="I24" t="n">
+      <c r="N24" t="n">
         <v>4.779</v>
       </c>
-      <c r="J24" t="n">
-        <v>0</v>
+      <c r="O24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" t="n">
+        <v>820.9979999999999</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>1055.4075</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2023-12-07T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Bancroft Hotel - Great Hall</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Bancroft</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>45</v>
+      </c>
+      <c r="E25" t="n">
         <v>1.4112</v>
       </c>
-      <c r="B25" t="n">
+      <c r="F25" t="n">
         <v>32.79149999999999</v>
       </c>
-      <c r="C25" t="n">
+      <c r="G25" t="n">
         <v>43.65899999999999</v>
       </c>
-      <c r="D25" t="n">
+      <c r="H25" t="n">
         <v>4.181624999999999</v>
       </c>
-      <c r="E25" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" t="n">
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="n">
+        <v>82.04332499999998</v>
+      </c>
+      <c r="K25" t="n">
         <v>0.3024000000000001</v>
       </c>
-      <c r="G25" t="n">
+      <c r="L25" t="n">
         <v>28.57545</v>
       </c>
-      <c r="H25" t="n">
+      <c r="M25" t="n">
         <v>93.55500000000001</v>
       </c>
-      <c r="I25" t="n">
+      <c r="N25" t="n">
         <v>0.71685</v>
       </c>
-      <c r="J25" t="n">
-        <v>0</v>
+      <c r="O25" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" t="n">
+        <v>123.1497</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>205.193025</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2023-12-14T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Bancroft Hotel - Great Hall</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Bancroft</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>26</v>
+      </c>
+      <c r="E26" t="n">
         <v>0.9318400000000002</v>
       </c>
-      <c r="B26" t="n">
+      <c r="F26" t="n">
         <v>21.6528</v>
       </c>
-      <c r="C26" t="n">
+      <c r="G26" t="n">
         <v>28.8288</v>
       </c>
-      <c r="D26" t="n">
+      <c r="H26" t="n">
         <v>2.7612</v>
       </c>
-      <c r="E26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" t="n">
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="n">
+        <v>54.17464</v>
+      </c>
+      <c r="K26" t="n">
         <v>0.11648</v>
       </c>
-      <c r="G26" t="n">
+      <c r="L26" t="n">
         <v>11.00684</v>
       </c>
-      <c r="H26" t="n">
+      <c r="M26" t="n">
         <v>36.036</v>
       </c>
-      <c r="I26" t="n">
+      <c r="N26" t="n">
         <v>0.27612</v>
       </c>
-      <c r="J26" t="n">
-        <v>0</v>
+      <c r="O26" t="n">
+        <v>0</v>
+      </c>
+      <c r="P26" t="n">
+        <v>47.43544</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>101.61008</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2023-04-18T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>SPIEKER FORUM</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>ACT</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>140</v>
+      </c>
+      <c r="E27" t="n">
         <v>5.3312</v>
       </c>
-      <c r="B27" t="n">
+      <c r="F27" t="n">
         <v>123.879</v>
       </c>
-      <c r="C27" t="n">
+      <c r="G27" t="n">
         <v>164.934</v>
       </c>
-      <c r="D27" t="n">
+      <c r="H27" t="n">
         <v>15.79725</v>
       </c>
-      <c r="E27" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" t="n">
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="n">
+        <v>309.94145</v>
+      </c>
+      <c r="K27" t="n">
         <v>0.4704</v>
       </c>
-      <c r="G27" t="n">
+      <c r="L27" t="n">
         <v>44.4507</v>
       </c>
-      <c r="H27" t="n">
+      <c r="M27" t="n">
         <v>145.53</v>
       </c>
-      <c r="I27" t="n">
+      <c r="N27" t="n">
         <v>1.1151</v>
       </c>
-      <c r="J27" t="n">
-        <v>0</v>
+      <c r="O27" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" t="n">
+        <v>191.5662</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>501.50765</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2023-04-27T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Deans Conference Room</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>ACT</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>60</v>
+      </c>
+      <c r="E28" t="n">
         <v>2.2848</v>
       </c>
-      <c r="B28" t="n">
+      <c r="F28" t="n">
         <v>53.09099999999999</v>
       </c>
-      <c r="C28" t="n">
+      <c r="G28" t="n">
         <v>70.68599999999999</v>
       </c>
-      <c r="D28" t="n">
+      <c r="H28" t="n">
         <v>6.77025</v>
       </c>
-      <c r="E28" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" t="n">
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>132.83205</v>
+      </c>
+      <c r="K28" t="n">
         <v>0.2016</v>
       </c>
-      <c r="G28" t="n">
+      <c r="L28" t="n">
         <v>19.0503</v>
       </c>
-      <c r="H28" t="n">
+      <c r="M28" t="n">
         <v>62.37</v>
       </c>
-      <c r="I28" t="n">
+      <c r="N28" t="n">
         <v>0.4778999999999999</v>
       </c>
-      <c r="J28" t="n">
-        <v>0</v>
+      <c r="O28" t="n">
+        <v>0</v>
+      </c>
+      <c r="P28" t="n">
+        <v>82.0998</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>214.93185</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2023-05-02T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>University Club</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Levy Restaurants</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>100</v>
+      </c>
+      <c r="E29" t="n">
         <v>2.24</v>
       </c>
-      <c r="B29" t="n">
+      <c r="F29" t="n">
         <v>52.05</v>
       </c>
-      <c r="C29" t="n">
+      <c r="G29" t="n">
         <v>69.3</v>
       </c>
-      <c r="D29" t="n">
+      <c r="H29" t="n">
         <v>6.637499999999999</v>
       </c>
-      <c r="E29" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" t="n">
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="n">
+        <v>130.2275</v>
+      </c>
+      <c r="K29" t="n">
         <v>1.12</v>
       </c>
-      <c r="G29" t="n">
+      <c r="L29" t="n">
         <v>105.835</v>
       </c>
-      <c r="H29" t="n">
+      <c r="M29" t="n">
         <v>346.5</v>
       </c>
-      <c r="I29" t="n">
+      <c r="N29" t="n">
         <v>2.655</v>
       </c>
-      <c r="J29" t="n">
-        <v>0</v>
+      <c r="O29" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" t="n">
+        <v>456.11</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>586.3375</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2023-05-19T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Haas School of Business Courtyard</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>ACT</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>1600</v>
+      </c>
+      <c r="E30" t="n">
         <v>50.17600000000001</v>
       </c>
-      <c r="B30" t="n">
+      <c r="F30" t="n">
         <v>1165.92</v>
       </c>
-      <c r="C30" t="n">
+      <c r="G30" t="n">
         <v>1552.32</v>
       </c>
-      <c r="D30" t="n">
+      <c r="H30" t="n">
         <v>148.68</v>
       </c>
-      <c r="E30" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" t="n">
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="n">
+        <v>2917.096</v>
+      </c>
+      <c r="K30" t="n">
         <v>10.752</v>
       </c>
-      <c r="G30" t="n">
+      <c r="L30" t="n">
         <v>1016.016</v>
       </c>
-      <c r="H30" t="n">
+      <c r="M30" t="n">
         <v>3326.4</v>
       </c>
-      <c r="I30" t="n">
+      <c r="N30" t="n">
         <v>25.488</v>
       </c>
-      <c r="J30" t="n">
-        <v>0</v>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" t="n">
+        <v>4378.656</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>7295.752</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2023-09-13T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Haas School of Business Courtyard</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>ACT</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>800</v>
+      </c>
+      <c r="E31" t="n">
         <v>28.672</v>
       </c>
-      <c r="B31" t="n">
+      <c r="F31" t="n">
         <v>666.24</v>
       </c>
-      <c r="C31" t="n">
+      <c r="G31" t="n">
         <v>887.04</v>
       </c>
-      <c r="D31" t="n">
+      <c r="H31" t="n">
         <v>84.95999999999999</v>
       </c>
-      <c r="E31" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" t="n">
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="n">
+        <v>1666.912</v>
+      </c>
+      <c r="K31" t="n">
         <v>3.584000000000001</v>
       </c>
-      <c r="G31" t="n">
+      <c r="L31" t="n">
         <v>338.672</v>
       </c>
-      <c r="H31" t="n">
+      <c r="M31" t="n">
         <v>1108.8</v>
       </c>
-      <c r="I31" t="n">
+      <c r="N31" t="n">
         <v>8.496</v>
       </c>
-      <c r="J31" t="n">
-        <v>0</v>
+      <c r="O31" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" t="n">
+        <v>1459.552</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>3126.464</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2023-09-13T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>SPIEKER FORUM</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>ACT</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>800</v>
+      </c>
+      <c r="E32" t="n">
         <v>30.464</v>
       </c>
-      <c r="B32" t="n">
+      <c r="F32" t="n">
         <v>707.88</v>
       </c>
-      <c r="C32" t="n">
+      <c r="G32" t="n">
         <v>942.4799999999999</v>
       </c>
-      <c r="D32" t="n">
+      <c r="H32" t="n">
         <v>90.27</v>
       </c>
-      <c r="E32" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" t="n">
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" t="n">
+        <v>1771.094</v>
+      </c>
+      <c r="K32" t="n">
         <v>2.688</v>
       </c>
-      <c r="G32" t="n">
+      <c r="L32" t="n">
         <v>254.004</v>
       </c>
-      <c r="H32" t="n">
+      <c r="M32" t="n">
         <v>831.5999999999999</v>
       </c>
-      <c r="I32" t="n">
+      <c r="N32" t="n">
         <v>6.371999999999999</v>
       </c>
-      <c r="J32" t="n">
-        <v>0</v>
+      <c r="O32" t="n">
+        <v>0</v>
+      </c>
+      <c r="P32" t="n">
+        <v>1094.664</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>2865.758</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2023-10-10T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>SPIEKER FORUM</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>ACT</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>120</v>
+      </c>
+      <c r="E33" t="n">
         <v>4.5696</v>
       </c>
-      <c r="B33" t="n">
+      <c r="F33" t="n">
         <v>106.182</v>
       </c>
-      <c r="C33" t="n">
+      <c r="G33" t="n">
         <v>141.372</v>
       </c>
-      <c r="D33" t="n">
+      <c r="H33" t="n">
         <v>13.5405</v>
       </c>
-      <c r="E33" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" t="n">
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>265.6641</v>
+      </c>
+      <c r="K33" t="n">
         <v>0.4032</v>
       </c>
-      <c r="G33" t="n">
+      <c r="L33" t="n">
         <v>38.1006</v>
       </c>
-      <c r="H33" t="n">
+      <c r="M33" t="n">
         <v>124.74</v>
       </c>
-      <c r="I33" t="n">
+      <c r="N33" t="n">
         <v>0.9557999999999999</v>
       </c>
-      <c r="J33" t="n">
-        <v>0</v>
+      <c r="O33" t="n">
+        <v>0</v>
+      </c>
+      <c r="P33" t="n">
+        <v>164.1996</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>429.8637</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2023-11-08T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>SPIEKER FORUM</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>ACT</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>180</v>
+      </c>
+      <c r="E34" t="n">
         <v>4.032000000000001</v>
       </c>
-      <c r="B34" t="n">
+      <c r="F34" t="n">
         <v>93.69</v>
       </c>
-      <c r="C34" t="n">
+      <c r="G34" t="n">
         <v>124.74</v>
       </c>
-      <c r="D34" t="n">
+      <c r="H34" t="n">
         <v>11.9475</v>
       </c>
-      <c r="E34" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" t="n">
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="n">
+        <v>234.4095</v>
+      </c>
+      <c r="K34" t="n">
         <v>2.016</v>
       </c>
-      <c r="G34" t="n">
+      <c r="L34" t="n">
         <v>190.503</v>
       </c>
-      <c r="H34" t="n">
+      <c r="M34" t="n">
         <v>623.6999999999999</v>
       </c>
-      <c r="I34" t="n">
+      <c r="N34" t="n">
         <v>4.779</v>
       </c>
-      <c r="J34" t="n">
-        <v>0</v>
+      <c r="O34" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" t="n">
+        <v>820.9979999999999</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>1055.4075</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2023-12-13T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>SPIEKER FORUM</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>ACT</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>160</v>
+      </c>
+      <c r="E35" t="n">
         <v>5.017600000000001</v>
       </c>
-      <c r="B35" t="n">
+      <c r="F35" t="n">
         <v>116.592</v>
       </c>
-      <c r="C35" t="n">
+      <c r="G35" t="n">
         <v>155.232</v>
       </c>
-      <c r="D35" t="n">
+      <c r="H35" t="n">
         <v>14.868</v>
       </c>
-      <c r="E35" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" t="n">
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="n">
+        <v>291.7096</v>
+      </c>
+      <c r="K35" t="n">
         <v>1.0752</v>
       </c>
-      <c r="G35" t="n">
+      <c r="L35" t="n">
         <v>101.6016</v>
       </c>
-      <c r="H35" t="n">
+      <c r="M35" t="n">
         <v>332.64</v>
       </c>
-      <c r="I35" t="n">
+      <c r="N35" t="n">
         <v>2.5488</v>
       </c>
-      <c r="J35" t="n">
-        <v>0</v>
+      <c r="O35" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" t="n">
+        <v>437.8656</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>729.5752</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="n">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2023-10-11T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Julia Morgan Hall UC Botanic Garden</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Slippery Fish</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>100</v>
+      </c>
+      <c r="E36" t="n">
         <v>3.584000000000001</v>
       </c>
-      <c r="B36" t="n">
+      <c r="F36" t="n">
         <v>83.28</v>
       </c>
-      <c r="C36" t="n">
+      <c r="G36" t="n">
         <v>110.88</v>
       </c>
-      <c r="D36" t="n">
+      <c r="H36" t="n">
         <v>10.62</v>
       </c>
-      <c r="E36" t="n">
-        <v>0</v>
-      </c>
-      <c r="F36" t="n">
+      <c r="I36" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" t="n">
+        <v>208.364</v>
+      </c>
+      <c r="K36" t="n">
         <v>0.4480000000000001</v>
       </c>
-      <c r="G36" t="n">
+      <c r="L36" t="n">
         <v>42.334</v>
       </c>
-      <c r="H36" t="n">
+      <c r="M36" t="n">
         <v>138.6</v>
       </c>
-      <c r="I36" t="n">
+      <c r="N36" t="n">
         <v>1.062</v>
       </c>
-      <c r="J36" t="n">
-        <v>0</v>
+      <c r="O36" t="n">
+        <v>0</v>
+      </c>
+      <c r="P36" t="n">
+        <v>182.444</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>390.808</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="n">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2023-05-19T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Chou Hall N340 / N344</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Slippery Fish</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>40</v>
+      </c>
+      <c r="E37" t="n">
         <v>1.5232</v>
       </c>
-      <c r="B37" t="n">
+      <c r="F37" t="n">
         <v>35.394</v>
       </c>
-      <c r="C37" t="n">
+      <c r="G37" t="n">
         <v>47.124</v>
       </c>
-      <c r="D37" t="n">
+      <c r="H37" t="n">
         <v>4.513500000000001</v>
       </c>
-      <c r="E37" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" t="n">
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>88.5547</v>
+      </c>
+      <c r="K37" t="n">
         <v>0.1344</v>
       </c>
-      <c r="G37" t="n">
+      <c r="L37" t="n">
         <v>12.7002</v>
       </c>
-      <c r="H37" t="n">
+      <c r="M37" t="n">
         <v>41.58000000000001</v>
       </c>
-      <c r="I37" t="n">
+      <c r="N37" t="n">
         <v>0.3185999999999999</v>
       </c>
-      <c r="J37" t="n">
-        <v>0</v>
+      <c r="O37" t="n">
+        <v>0</v>
+      </c>
+      <c r="P37" t="n">
+        <v>54.7332</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>143.2879</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2023-05-16T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Chou Hall N340 / N344</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Slippery Fish</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>35</v>
+      </c>
+      <c r="E38" t="n">
         <v>1.3328</v>
       </c>
-      <c r="B38" t="n">
+      <c r="F38" t="n">
         <v>30.96974999999999</v>
       </c>
-      <c r="C38" t="n">
+      <c r="G38" t="n">
         <v>41.2335</v>
       </c>
-      <c r="D38" t="n">
+      <c r="H38" t="n">
         <v>3.9493125</v>
       </c>
-      <c r="E38" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" t="n">
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="n">
+        <v>77.48536249999999</v>
+      </c>
+      <c r="K38" t="n">
         <v>0.1176</v>
       </c>
-      <c r="G38" t="n">
+      <c r="L38" t="n">
         <v>11.112675</v>
       </c>
-      <c r="H38" t="n">
+      <c r="M38" t="n">
         <v>36.3825</v>
       </c>
-      <c r="I38" t="n">
+      <c r="N38" t="n">
         <v>0.278775</v>
       </c>
-      <c r="J38" t="n">
-        <v>0</v>
+      <c r="O38" t="n">
+        <v>0</v>
+      </c>
+      <c r="P38" t="n">
+        <v>47.89155</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>125.3769125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
incomplete food waste code. may not work, rough draft. test in the morning and fix
</commit_message>
<xml_diff>
--- a/haas/output_csv/haas_emissions_report.xlsx
+++ b/haas/output_csv/haas_emissions_report.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="transportation" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="food_waste" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2694,4 +2695,22 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>